<commit_message>
updated the xcel file with python code
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/PythonCodeInput.xlsx
+++ b/src/test/resources/exceldata/PythonCodeInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uthik\git\DS_AlgoVer1\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6251DA2A-0EAD-49F0-8A11-3008334BE8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D009F0-A157-48C3-AA38-3A54DF50EE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13200" yWindow="8235" windowWidth="32340" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pythonCode" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,19 @@
     <t>pythoncode</t>
   </si>
   <si>
-    <t>print("hello")</t>
+    <t>pythonCode</t>
   </si>
   <si>
-    <t>print(hello")</t>
+    <t>num1=7
+num2=9
+sum=num1+num2
+print("The sum of {0} and {1} is {2}" .format(num1,num2,sum))</t>
   </si>
   <si>
-    <t>pythonCode</t>
+    <t>num1=7
+num2=9
+sum=num1+num2
+print("The sum is" sum)</t>
   </si>
 </sst>
 </file>
@@ -73,8 +79,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,7 +367,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,14 +380,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -401,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>